<commit_message>
Implementazione filtri Sfera 4.0
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0_NR_AZ.xlsx
+++ b/docs/tp/Sfera_4.0_NR_AZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3031C9-47CD-4F5C-AD3E-8CE57EC8769E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1DD176-018B-4775-B564-966A166BA0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -210,6 +210,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -495,7 +498,7 @@
   <dimension ref="A1:Q1489"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,24 +586,24 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="J4" t="s">
@@ -609,39 +612,39 @@
     </row>
     <row r="5" spans="1:10" ht="114.75">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="25.5">
       <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J6" t="s">
@@ -650,18 +653,18 @@
     </row>
     <row r="7" spans="1:10" ht="102">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="38.25">
       <c r="A8" s="3"/>

</xml_diff>